<commit_message>
Carpeta 14. Escaleta 9 y otros pequeños...
Carpeta 14. Escaleta 9 y otros pequeños...
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion10/Escaleta_CS_06_10_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion10/Escaleta_CS_06_10_CO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasSociales\fuentes\contenidos\grado06\guion10\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15508" windowHeight="7200"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15510" windowHeight="7200"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -694,7 +689,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -710,6 +705,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -741,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -778,14 +779,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,7 +851,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -882,7 +886,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1094,81 +1098,81 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:U121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.86328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.3984375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="34.1328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="32.86328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.86328125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="24.86328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.86328125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="18.265625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="30.265625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="18.86328125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="21.59765625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="13.86328125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="15.59765625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="29.265625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="21.59765625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="16.1328125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="16.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.73046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="30.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="29.28515625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="21.5703125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="11.3984375" style="3"/>
+    <col min="22" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="22"/>
+      <c r="N1" s="20"/>
       <c r="O1" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="22" t="s">
         <v>116</v>
       </c>
       <c r="Q1" s="21" t="s">
@@ -1187,19 +1191,19 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
+    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
       <c r="M2" s="15" t="s">
         <v>92</v>
       </c>
@@ -1214,7 +1218,7 @@
       <c r="T2" s="21"/>
       <c r="U2" s="21"/>
     </row>
-    <row r="3" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -1273,7 +1277,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
@@ -1330,7 +1334,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -1385,7 +1389,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -1440,7 +1444,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -1497,7 +1501,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -1554,7 +1558,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1611,7 +1615,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
@@ -1647,7 +1651,7 @@
         <v>8</v>
       </c>
       <c r="M10" s="6"/>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="23" t="s">
         <v>34</v>
       </c>
       <c r="O10" s="7"/>
@@ -1670,7 +1674,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -1706,7 +1710,7 @@
         <v>8</v>
       </c>
       <c r="M11" s="6"/>
-      <c r="N11" s="6" t="s">
+      <c r="N11" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O11" s="7"/>
@@ -1729,7 +1733,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
@@ -1786,7 +1790,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
@@ -1845,7 +1849,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
@@ -1902,7 +1906,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="31.7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>18</v>
       </c>
@@ -1957,7 +1961,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
@@ -2014,7 +2018,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="43" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>18</v>
       </c>
@@ -2069,7 +2073,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
@@ -2124,7 +2128,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
@@ -2181,7 +2185,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -2238,7 +2242,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
@@ -2295,7 +2299,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>18</v>
       </c>
@@ -2332,7 +2336,7 @@
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
     </row>
-    <row r="23" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>18</v>
       </c>
@@ -2366,7 +2370,7 @@
         <v>8</v>
       </c>
       <c r="M23" s="6"/>
-      <c r="N23" s="6" t="s">
+      <c r="N23" s="23" t="s">
         <v>32</v>
       </c>
       <c r="O23" s="7"/>
@@ -2389,7 +2393,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>18</v>
       </c>
@@ -2417,7 +2421,7 @@
         <v>8</v>
       </c>
       <c r="M24" s="6"/>
-      <c r="N24" s="6" t="s">
+      <c r="N24" s="23" t="s">
         <v>53</v>
       </c>
       <c r="O24" s="7" t="s">
@@ -2442,7 +2446,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="I25" s="4"/>
       <c r="K25" s="4"/>
@@ -2450,7 +2454,7 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
-    <row r="26" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="I26" s="4"/>
       <c r="K26" s="4"/>
@@ -2458,7 +2462,7 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
     </row>
-    <row r="27" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="I27" s="4"/>
       <c r="K27" s="4"/>
@@ -2466,7 +2470,7 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
     </row>
-    <row r="28" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="I28" s="4"/>
       <c r="K28" s="4"/>
@@ -2474,7 +2478,7 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
     </row>
-    <row r="29" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="I29" s="4"/>
       <c r="K29" s="4"/>
@@ -2482,7 +2486,7 @@
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
     </row>
-    <row r="30" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="I30" s="4"/>
       <c r="K30" s="4"/>
@@ -2490,7 +2494,7 @@
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
     </row>
-    <row r="31" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="I31" s="4"/>
       <c r="K31" s="4"/>
@@ -2498,7 +2502,7 @@
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
     </row>
-    <row r="32" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="I32" s="4"/>
       <c r="K32" s="4"/>
@@ -2506,7 +2510,7 @@
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
     </row>
-    <row r="33" spans="1:14" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="I33" s="4"/>
       <c r="K33" s="4"/>
@@ -2514,7 +2518,7 @@
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
     </row>
-    <row r="34" spans="1:14" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="I34" s="4"/>
       <c r="K34" s="4"/>
@@ -2522,7 +2526,7 @@
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
     </row>
-    <row r="35" spans="1:14" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="I35" s="4"/>
       <c r="K35" s="4"/>
@@ -2530,7 +2534,7 @@
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
     </row>
-    <row r="36" spans="1:14" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="I36" s="4"/>
       <c r="K36" s="4"/>
@@ -2538,7 +2542,7 @@
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
     </row>
-    <row r="37" spans="1:14" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="I37" s="4"/>
       <c r="K37" s="4"/>
@@ -2546,7 +2550,7 @@
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
     </row>
-    <row r="38" spans="1:14" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="I38" s="4"/>
       <c r="K38" s="4"/>
@@ -2554,7 +2558,7 @@
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
     </row>
-    <row r="39" spans="1:14" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="I39" s="4"/>
       <c r="K39" s="4"/>
@@ -2562,7 +2566,7 @@
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
     </row>
-    <row r="40" spans="1:14" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="I40" s="4"/>
       <c r="K40" s="4"/>
@@ -2570,7 +2574,7 @@
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
     </row>
-    <row r="41" spans="1:14" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="I41" s="4"/>
       <c r="K41" s="4"/>
@@ -2578,193 +2582,199 @@
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>117</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -2779,12 +2789,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I41">
@@ -2841,27 +2845,27 @@
       <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.86328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.86328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.73046875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" style="1"/>
-    <col min="14" max="14" width="24.265625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="69.86328125" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.3984375" style="1"/>
+    <col min="13" max="13" width="11.42578125" style="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="69.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2878,7 +2882,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2902,7 +2906,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -2921,7 +2925,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -2940,7 +2944,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2956,7 +2960,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -2973,7 +2977,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -2990,7 +2994,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -3005,7 +3009,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -3020,7 +3024,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -3035,7 +3039,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -3050,7 +3054,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -3065,7 +3069,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -3080,7 +3084,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -3095,7 +3099,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -3110,7 +3114,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -3125,7 +3129,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1" t="s">
@@ -3139,7 +3143,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1" t="s">
@@ -3153,7 +3157,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1" t="s">
@@ -3167,7 +3171,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1" t="s">
@@ -3181,7 +3185,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -3196,7 +3200,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -3211,7 +3215,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -3226,7 +3230,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -3241,7 +3245,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -3256,7 +3260,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -3271,7 +3275,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -3286,7 +3290,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:12" ht="15.95" x14ac:dyDescent="0.5">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -3301,7 +3305,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -3316,7 +3320,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -3331,7 +3335,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -3346,7 +3350,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -3361,7 +3365,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -3376,7 +3380,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -3391,7 +3395,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -3406,7 +3410,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -3421,7 +3425,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -3436,7 +3440,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -3451,7 +3455,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -3466,7 +3470,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -3481,7 +3485,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -3496,7 +3500,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -3511,7 +3515,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -3526,7 +3530,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -3541,7 +3545,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -3556,7 +3560,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -3571,7 +3575,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -3586,7 +3590,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -3601,7 +3605,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -3613,7 +3617,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -3625,7 +3629,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -3638,7 +3642,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -3651,7 +3655,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -3664,7 +3668,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -3677,7 +3681,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -3690,7 +3694,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -3703,7 +3707,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -3716,7 +3720,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -3729,7 +3733,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -3742,7 +3746,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -3755,7 +3759,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -3768,7 +3772,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -3781,7 +3785,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -3794,7 +3798,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -3807,7 +3811,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -3820,7 +3824,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -3833,7 +3837,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -3846,7 +3850,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -3859,7 +3863,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -3872,7 +3876,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -3885,7 +3889,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -3899,7 +3903,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -3913,7 +3917,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -3927,7 +3931,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -3941,7 +3945,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3955,7 +3959,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3969,7 +3973,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -3983,7 +3987,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -3997,7 +4001,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -4011,7 +4015,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -4025,7 +4029,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -4039,7 +4043,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -4053,7 +4057,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -4067,7 +4071,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -4081,7 +4085,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -4095,7 +4099,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -4109,7 +4113,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -4123,7 +4127,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -4137,7 +4141,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -4151,7 +4155,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -4165,7 +4169,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -4179,7 +4183,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -4193,7 +4197,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -4207,7 +4211,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -4221,7 +4225,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -4235,7 +4239,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -4249,7 +4253,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -4263,7 +4267,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -4277,7 +4281,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -4291,7 +4295,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -4305,7 +4309,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -4319,7 +4323,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -4333,7 +4337,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -4347,7 +4351,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -4361,7 +4365,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -4375,7 +4379,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -4389,7 +4393,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -4403,7 +4407,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -4417,7 +4421,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -4431,7 +4435,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -4445,7 +4449,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -4459,7 +4463,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -4473,7 +4477,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -4487,7 +4491,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -4501,7 +4505,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -4515,7 +4519,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -4529,7 +4533,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -4543,7 +4547,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -4557,7 +4561,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -4571,7 +4575,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -4585,7 +4589,7 @@
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -4599,7 +4603,7 @@
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -4613,7 +4617,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -4627,7 +4631,7 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -4641,7 +4645,7 @@
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -4655,7 +4659,7 @@
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -4669,7 +4673,7 @@
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -4683,7 +4687,7 @@
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -4697,7 +4701,7 @@
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -4711,7 +4715,7 @@
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -4725,7 +4729,7 @@
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -4739,7 +4743,7 @@
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -4753,7 +4757,7 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>

</xml_diff>